<commit_message>
Updating therm, fixing vocab discrepancies
</commit_message>
<xml_diff>
--- a/Projects/iRL/Parameters/config.xlsx
+++ b/Projects/iRL/Parameters/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0. ProtonDrive\Other computers\DESKTOP-PR117J6\Software\Peira\Projects\iRL\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613313ED-A8D0-40CA-BB7B-44C6FEC9536D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7085B3-5394-4519-B16F-D5CB2884BEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,27 +163,6 @@
     <t>Signal Heater Off __________ Off Signal Failed</t>
   </si>
   <si>
-    <t>Heater was previously on __________ Heater On</t>
-  </si>
-  <si>
-    <t>On Signal Succeeded ___________ Heater On</t>
-  </si>
-  <si>
-    <t>On Signal Failed ___________ Heater On</t>
-  </si>
-  <si>
-    <t>Off Signal Succeeded ___________ Heater On</t>
-  </si>
-  <si>
-    <t>Off Signal Failed ___________ Heater On</t>
-  </si>
-  <si>
-    <t>Heater On ___________ Minimize Running Time</t>
-  </si>
-  <si>
-    <t>Heater On ___________ Maintain Ideal Temperature (current level)</t>
-  </si>
-  <si>
     <t>Minimize Running Time ___________ Minimize Cost</t>
   </si>
   <si>
@@ -289,9 +268,6 @@
     <t>caseText</t>
   </si>
   <si>
-    <t>We are modeling a &lt;mark&gt;heating controller&lt;/mark&gt;. The heating controller's purpose is to &lt;mark&gt;maintain optimal room temperature&lt;/mark&gt; at all times. To do so, it sends periodic signals that turn on or off an electric heater. Specifically the controller may choose to send to &lt;mark&gt;signal the heater on&lt;/mark&gt; or &lt;mark&gt;signal heater off&lt;/mark&gt;. These signals are sent wirelessly to the heater, so they are not always received. Thus, when an on signal is sent the outcome can be that the &lt;mark&gt;On Signal Succeeded&lt;/mark&gt; or that the &lt;mark&gt;On Signal Failed&lt;/mark&gt;. Likewise the outcome of an off signal can be &lt;mark&gt;Off Signal Succeeded&lt;/mark&gt; or &lt;mark&gt;Off Signal Failed&lt;/mark&gt;. Whether &lt;mark&gt;Heater is On&lt;/mark&gt; is eventually true depends on which of those four outcomes comes about as well as whether &lt;mark&gt;Heater was previously On&lt;/mark&gt;. &lt;BR&gt;&lt;BR&gt; The heating controller aims at maintaining optimal room temperature while &lt;mark&gt;minimizing cost&lt;/mark&gt; and &lt;mark&gt;maximizing comfort&lt;/mark&gt;. To minimize cost the controller needs to minimize running time, while to maximize comfort the controller needs to ensure that the &lt;mark&gt;ideal temperature is maintained&lt;/mark&gt;. Whether ideal temperature is maintained, however, depends on (a) the extend to which the &lt;mark&gt;ideal temperature was maintained at the previous state&lt;/mark&gt; (b) whether the heater is on.</t>
-  </si>
-  <si>
     <t>xXFA-QvdyDU</t>
   </si>
   <si>
@@ -439,9 +415,6 @@
     <t>Signal Heater Off __________ Off Signal Succeeded, Off Signal Failed</t>
   </si>
   <si>
-    <t>Temperature Controlled __________ Signal Heater On and Signal Heater Off</t>
-  </si>
-  <si>
     <t>pre</t>
   </si>
   <si>
@@ -670,9 +643,6 @@
     <t>Maintain Ideal Temperature in the previous stage ___________ Maintain Ideal Temperature (current stage)</t>
   </si>
   <si>
-    <t>Controller __________ Have Temperature Controlled</t>
-  </si>
-  <si>
     <t>tq5Jlj5PIp4</t>
   </si>
   <si>
@@ -710,6 +680,36 @@
   </si>
   <si>
     <t>An outcome of an action attempt</t>
+  </si>
+  <si>
+    <t>We are modeling a &lt;mark&gt;temperature controller&lt;/mark&gt;.  The controller's purpose is &lt;mark&gt;to have the temperature of a room controlled&lt;/mark&gt; at all times. To do so, it sends periodic signals that turn on or off the heater. Specifically the controller may choose to &lt;mark&gt;send an on signal&lt;/mark&gt; or to &lt;mark&gt;send an off signal&lt;/mark&gt; to the heater. These signals are sent wirelessly to the heater, so they are not always received. Thus, when an on signal is sent the outcome can be that the &lt;mark&gt;on-signal succeeded&lt;/mark&gt; or that the &lt;mark&gt;on-signal failed&lt;/mark&gt;  Likewise the outcome of an off signal can be &lt;mark&gt;off-signal succeeded&lt;/mark&gt; or &lt;mark&gt;off-signal failed&lt;/mark&gt;  Whether that &lt;mark&gt;heater is on&lt;/mark&gt; is eventually true depends on which of those four outcomes comes about as well as whether the &lt;mark&gt;heater was previously on&lt;/mark&gt;  The temperature controller sends on and off signals aimed at satisfying some high-level objectives of the occupants of the room. One is to &lt;mark&gt;maximize comfort&lt;/mark&gt; via &lt;mark&gt;maintaining the ideal temperature&lt;/mark&gt; in the room. Maintaining the ideal temperature depends on whether the &lt;mark&gt;ideal temperature was maintained in the previous stage&lt;/mark&gt; and the heater was on or off meanwhile. At the same time the controller wants to ensure that the heater does not stay unnecessarily on for a long period of time. It does that aimed at &lt;mark&gt;minimizing cost&lt;/mark&gt;.</t>
+  </si>
+  <si>
+    <t>Have Temperature Controlled __________ Send On Signal, Send Off Signal</t>
+  </si>
+  <si>
+    <t>Heater was previously on __________ Heater Is On</t>
+  </si>
+  <si>
+    <t>On Signal Succeeded ___________ Heater Is On</t>
+  </si>
+  <si>
+    <t>On Signal Failed ___________ Heater Is On</t>
+  </si>
+  <si>
+    <t>Off Signal Succeeded ___________ Heater Is On</t>
+  </si>
+  <si>
+    <t>Off Signal Failed ___________ Heater Is On</t>
+  </si>
+  <si>
+    <t>Heater Is On ___________ Minimize Running Time</t>
+  </si>
+  <si>
+    <t>Heater Is On ___________ Maintain Ideal Temperature (current level)</t>
+  </si>
+  <si>
+    <t>Temperature Controller __________ Have Temperature Controlled</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,10 +1158,10 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1184,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1214,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -1244,7 +1244,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1274,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -1304,10 +1304,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -1334,10 +1334,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="H7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -1364,10 +1364,10 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -1394,10 +1394,10 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -1427,7 +1427,7 @@
         <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1454,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -1484,7 +1484,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1514,7 +1514,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1574,7 +1574,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>130</v>
+        <v>212</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1658,10 +1658,10 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -1685,7 +1685,7 @@
         <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -1712,10 +1712,10 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H20" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -1739,7 +1739,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -1766,10 +1766,10 @@
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>213</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -1796,10 +1796,10 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>214</v>
       </c>
       <c r="H23" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -1826,10 +1826,10 @@
         <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>215</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -1856,10 +1856,10 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>216</v>
       </c>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
@@ -1886,10 +1886,10 @@
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>217</v>
       </c>
       <c r="H26" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -1916,10 +1916,10 @@
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
+        <v>218</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -1946,7 +1946,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -1976,7 +1976,7 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
@@ -2000,20 +2000,17 @@
         <v>9</v>
       </c>
       <c r="E30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
-        <v>contributes to</v>
+        <v>positively contributes to</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2033,17 +2030,17 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
-        <v>contributes to</v>
+        <v>positively contributes to</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2063,13 +2060,13 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="H32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ref="I32:I58" si="1">VLOOKUP(H32,iRL,2,FALSE)</f>
@@ -2078,10 +2075,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2096,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H33" t="s">
         <v>19</v>
@@ -2108,10 +2105,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2126,7 +2123,7 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
@@ -2138,10 +2135,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2156,7 +2153,7 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H35" t="s">
         <v>20</v>
@@ -2168,10 +2165,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -2186,7 +2183,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
@@ -2198,10 +2195,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -2216,7 +2213,7 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H37" t="s">
         <v>20</v>
@@ -2228,10 +2225,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -2246,7 +2243,7 @@
         <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
@@ -2258,10 +2255,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -2276,10 +2273,10 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H39" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="1"/>
@@ -2288,10 +2285,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -2306,10 +2303,10 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H40" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="1"/>
@@ -2318,10 +2315,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B41" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -2336,10 +2333,10 @@
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H41" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -2348,10 +2345,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -2366,10 +2363,10 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H42" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="1"/>
@@ -2378,10 +2375,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -2396,10 +2393,10 @@
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H43" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="1"/>
@@ -2408,10 +2405,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B44" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -2426,7 +2423,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -2438,10 +2435,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C45">
         <v>13</v>
@@ -2456,7 +2453,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2468,10 +2465,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -2486,7 +2483,7 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -2498,10 +2495,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -2516,10 +2513,10 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="H47" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
@@ -2528,10 +2525,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C48">
         <v>16</v>
@@ -2546,10 +2543,10 @@
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H48" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="1"/>
@@ -2558,10 +2555,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2576,7 +2573,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H49" t="s">
         <v>12</v>
@@ -2588,10 +2585,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -2606,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
@@ -2618,10 +2615,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -2636,10 +2633,10 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H51" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="1"/>
@@ -2648,10 +2645,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2666,10 +2663,10 @@
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H52" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="1"/>
@@ -2678,10 +2675,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -2696,10 +2693,10 @@
         <v>5</v>
       </c>
       <c r="G53" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H53" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -2708,10 +2705,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -2726,10 +2723,10 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H54" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
@@ -2738,10 +2735,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C55">
         <v>7</v>
@@ -2756,10 +2753,10 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H55" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
@@ -2768,10 +2765,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C56">
         <v>8</v>
@@ -2786,7 +2783,7 @@
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
@@ -2798,10 +2795,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C57">
         <v>9</v>
@@ -2816,10 +2813,10 @@
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="H57" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="1"/>
@@ -2828,10 +2825,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -2846,10 +2843,10 @@
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H58" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="1"/>
@@ -2866,7 +2863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A67578-F426-48F2-87A8-25344D20072D}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2882,28 +2879,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2920,10 +2917,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -2946,10 +2943,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2972,10 +2969,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -2986,10 +2983,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -2998,10 +2995,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -3012,10 +3009,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
@@ -3024,10 +3021,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -3038,11 +3035,11 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
@@ -3050,10 +3047,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -3067,7 +3064,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -3076,10 +3073,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -3102,10 +3099,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -3119,7 +3116,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -3128,10 +3125,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -3142,10 +3139,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3154,10 +3151,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F11" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -3171,7 +3168,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3180,10 +3177,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -3197,7 +3194,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3206,10 +3203,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -3220,10 +3217,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3232,10 +3229,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F14" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -3246,10 +3243,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3258,10 +3255,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F15" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3272,10 +3269,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3284,10 +3281,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -3298,10 +3295,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3310,10 +3307,10 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -3327,7 +3324,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -3336,10 +3333,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F18" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -3350,10 +3347,10 @@
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -3362,10 +3359,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G19" s="6" t="b">
         <v>1</v>
@@ -3382,16 +3379,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G20" s="6" t="b">
         <v>0</v>
@@ -3408,16 +3405,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G21" s="6" t="b">
         <v>0</v>
@@ -3434,16 +3431,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G22" s="6" t="b">
         <v>0</v>
@@ -3457,19 +3454,19 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G23" s="6" t="b">
         <v>0</v>
@@ -3486,16 +3483,16 @@
         <v>6</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G24" s="6" t="b">
         <v>0</v>
@@ -3506,22 +3503,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G25" s="6" t="b">
         <v>1</v>
@@ -3535,19 +3532,19 @@
         <v>12</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G26" s="6" t="b">
         <v>1</v>
@@ -3561,19 +3558,19 @@
         <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G27" s="6" t="b">
         <v>1</v>
@@ -3584,22 +3581,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="G28" s="6" t="b">
         <v>1</v>
@@ -3613,19 +3610,19 @@
         <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="G29" s="6" t="b">
         <v>1</v>
@@ -3636,22 +3633,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G30" s="6" t="b">
         <v>1</v>
@@ -3685,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3713,7 +3710,7 @@
         <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3741,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3769,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3797,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3825,7 +3822,7 @@
         <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3853,7 +3850,7 @@
         <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3881,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3909,12 +3906,12 @@
         <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
@@ -3937,12 +3934,12 @@
         <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -3965,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4018,43 +4015,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4062,63 +4059,63 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="K2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="L2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="M2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4137,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77FB8ED-296C-4040-BCEE-A5690B45B944}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,19 +4151,19 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>24</v>
@@ -4180,16 +4177,16 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
+        <v>211</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G2" s="3" t="b">
         <v>1</v>
@@ -4197,19 +4194,19 @@
     </row>
     <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -4236,71 +4233,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Adding image XMLs for Manufactuere case (initial)
</commit_message>
<xml_diff>
--- a/Projects/iRL/Parameters/config.xlsx
+++ b/Projects/iRL/Parameters/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0. ProtonDrive\Other computers\DESKTOP-PR117J6\Software\Peira\Projects\iRL\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Private\Others\Software\Peira\Projects\iRL\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12D5CDA-E32A-45FB-8CFF-830ED1FC163A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B28C95A-C2EF-4B26-8EEF-D4F3A357710C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -268,9 +268,6 @@
     <t>caseText</t>
   </si>
   <si>
-    <t>xXFA-QvdyDU</t>
-  </si>
-  <si>
     <t>iRL_auth</t>
   </si>
   <si>
@@ -709,18 +706,19 @@
     <t>Acquire Parts ___________ Have the Engine Assembled</t>
   </si>
   <si>
-    <t>Powerful Engines Inc. is an &lt;mark&gt;Engine Manufacturer&lt;/mark&gt; located in North America. They design and assemble small combustion engines for a small customer list of power tool manufacturers, with many of whom they have long-term contracts. Every time one of those customers places an order, our Engine Manufacturer needs to &lt;mark&gt;Have that Order Fulfilled&lt;/mark&gt; by a strict deadline. To do so they need to do two things. First they need to &lt;mark&gt;Acquire the Parts&lt;/mark&gt; necessary for assembling the engine from a variety of suppliers. The parts may be &lt;mark&gt;Acquired in Time&lt;/mark&gt;, may be &lt;mark&gt;Acquired Late&lt;/mark&gt; or they may be &lt;mark&gt;Never Acquired&lt;/mark&gt; before the absolute deadline. In the latter case the &lt;mark&gt;Order is Canceled&lt;/mark&gt; as the company cannot honor the time commitment to the client. According to the contract a &lt;mark&gt;Penalty is Issued&lt;/mark&gt; for two consecutive cancellations. In other words a &lt;mark&gt;Penalty is Issued&lt;/mark&gt; if the order is cancelled and the &lt;mark&gt;Order was Cancelled&lt;/mark&gt; in the previous instance as well. 
-Once the parts are acquired, the manufacturer is then able to &lt;mark&gt;Have the Engine Assembled&lt;/mark&gt;. They have two options here. They can &lt;mark&gt;Assemble the Engine in House&lt;/mark&gt; using their specialized high-quality facilities, or they can choose to &lt;mark&gt;Outsource Assembly&lt;/mark&gt; in order to cut costs for the customer.  Although choosing to Outsource Assembly is cheaper, it is also a gamble: the result may be &lt;mark&gt;Good Construction Quality&lt;/mark&gt; or &lt;mark&gt;Bad Construction Quality&lt;/mark&gt;. 
-The manufacturer is very conscious of their &lt;mark&gt;Reputation&lt;/mark&gt;. Their Reputation level after dealing with an order, depends on the level of Reputation they already enjoyed before, minus the loss in reputation they suffer if the &lt;mark&gt;Order is Cancelled&lt;/mark&gt; or the assembly results in &lt;mark&gt;Bad Construction Quality&lt;/mark&gt;, but plus the boost in reputation they enjoy when the result is actually of &lt;mark&gt;Good Construction Quality&lt;/mark&gt;.</t>
-  </si>
-  <si>
     <t>paste0('&lt;h3&gt;Exercise 1&lt;/h3&gt; The passage below describes the operation of an Engine Manufacturer. Read the passage. Then you will be asked to classify the &lt;mark&gt;highlighted expressions&lt;/mark&gt; to one of the concepts or relationships presented in the video presentation ', summary, '. &lt;BR&gt;&lt;BR&gt;')</t>
   </si>
   <si>
-    <t>paste0('&lt;h2&gt;Classification Exercise 2: Engine Manufacturer&lt;/h2&gt;Please watch the following video with directions.  If embedded video does not load, you can  &lt;a href="https://www.google.com" target="_blank"&gt;watch it directly on Youtube&lt;/a&gt;')</t>
-  </si>
-  <si>
     <t>paste0('&lt;h2&gt;Classification Exercise 1: Temperature Controller&lt;/h2&gt;Please watch the following video with directions.  If embedded video does not load, you can  &lt;a href="https://www.youtube.com/watch?v=sYgBjZzdxZM&amp;t=119s" target="_blank"&gt;watch it directly on Youtube&lt;/a&gt;')</t>
+  </si>
+  <si>
+    <t>Powerful Engines Inc. is an &lt;mark&gt;Engine Manufacturer&lt;/mark&gt; located in North America. They design and assemble small combustion engines for a small customer list of power tool manufacturers, with many of whom they have long-term contracts. Every time one of those customers places an order, our Engine Manufacturer needs to &lt;mark&gt;Have that Order Fulfilled&lt;/mark&gt; by a strict deadline. To do so they need to do two things. First they need to &lt;mark&gt;Acquire the Parts&lt;/mark&gt; necessary for assembling the engine from a variety of suppliers. The parts may be &lt;mark&gt;Acquired in Time&lt;/mark&gt;, may be &lt;mark&gt;Acquired Late&lt;/mark&gt; or they may be &lt;mark&gt;Never Acquired&lt;/mark&gt; before the absolute deadline. In the latter case the &lt;mark&gt;Order is Canceled&lt;/mark&gt; as the company cannot honor the time commitment to the client. According to the contract a &lt;mark&gt;Penalty is Issued&lt;/mark&gt; for two consecutive cancellations. In other words a &lt;mark&gt;Penalty is Issued&lt;/mark&gt; if the order is cancelled and the &lt;mark&gt;Order was Cancelled&lt;/mark&gt; in the previous instance as well. &lt;BR&gt;&lt;BR&gt; Once the parts are acquired, the manufacturer is then able to &lt;mark&gt;Have the Engine Assembled&lt;/mark&gt;. They have two options here. They can &lt;mark&gt;Assemble the Engine in House&lt;/mark&gt; using their specialized high-quality facilities, or they can choose to &lt;mark&gt;Outsource Assembly&lt;/mark&gt; in order to cut costs for the customer.  Although choosing to Outsource Assembly is cheaper, it is also a gamble: the result may be &lt;mark&gt;Good Construction Quality&lt;/mark&gt; or &lt;mark&gt;Bad Construction Quality&lt;/mark&gt;. &lt;BR&gt;&lt;BR&gt; The manufacturer is very conscious of their &lt;mark&gt;Reputation&lt;/mark&gt;. Their Reputation level after dealing with an order, depends on the level of Reputation they already enjoyed before, minus the loss in reputation they suffer if the &lt;mark&gt;Order is Cancelled&lt;/mark&gt; or the assembly results in &lt;mark&gt;Bad Construction Quality&lt;/mark&gt;, but plus the boost in reputation they enjoy when the result is actually of &lt;mark&gt;Good Construction Quality&lt;/mark&gt;.</t>
+  </si>
+  <si>
+    <t>paste0('&lt;h2&gt;Classification Exercise 2: Engine Manufacturer&lt;/h2&gt;Please watch the following video with directions.  If embedded video does not load, you can  &lt;a href="https://youtu.be/vcqtxLosHhU" target="_blank"&gt;watch it directly on Youtube&lt;/a&gt;')</t>
+  </si>
+  <si>
+    <t>vcqtxLosHhU</t>
   </si>
 </sst>
 </file>
@@ -792,7 +790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -811,6 +809,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1093,7 +1094,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
+  <wetp:taskpane dockstate="right" visibility="0" width="401" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
@@ -1145,21 +1146,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1182,13 +1183,13 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1218,7 +1219,7 @@
         <v>Actor</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1238,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -1248,7 +1249,7 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1278,7 +1279,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1298,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -1308,7 +1309,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1328,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
         <v>45</v>
@@ -1338,7 +1339,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
         <v>45</v>
@@ -1368,7 +1369,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H8" t="s">
         <v>45</v>
@@ -1398,7 +1399,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H9" t="s">
         <v>45</v>
@@ -1428,7 +1429,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -1488,7 +1489,7 @@
         <v>Pre-Effect</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1518,7 +1519,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1538,7 +1539,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1548,7 +1549,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1598,7 +1599,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -1608,7 +1609,7 @@
         <v>Pre-Quality</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1638,7 +1639,7 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H18" t="s">
         <v>44</v>
@@ -1692,7 +1693,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1716,7 +1717,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1736,7 +1737,7 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H20" t="s">
         <v>44</v>
@@ -1746,7 +1747,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>4</v>
       </c>
       <c r="G22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H22" t="s">
         <v>42</v>
@@ -1800,7 +1801,7 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>5</v>
       </c>
       <c r="G23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H23" t="s">
         <v>43</v>
@@ -1830,7 +1831,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H24" t="s">
         <v>43</v>
@@ -1860,7 +1861,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1880,7 +1881,7 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H25" t="s">
         <v>43</v>
@@ -1890,7 +1891,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1910,7 +1911,7 @@
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H26" t="s">
         <v>43</v>
@@ -1920,7 +1921,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H27" t="s">
         <v>51</v>
@@ -1950,7 +1951,7 @@
         <v>negatively contributes to</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -1980,7 +1981,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
@@ -2010,7 +2011,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>positively contributes to</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>positively contributes to</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2087,22 +2088,22 @@
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ref="I32:I58" si="1">VLOOKUP(H32,iRL,2,FALSE)</f>
         <v>wants to</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2117,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H33" t="s">
         <v>19</v>
@@ -2127,12 +2128,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2147,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
@@ -2157,12 +2158,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2177,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H35" t="s">
         <v>20</v>
@@ -2187,12 +2188,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -2207,7 +2208,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
@@ -2217,12 +2218,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -2237,7 +2238,7 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H37" t="s">
         <v>20</v>
@@ -2247,12 +2248,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B38" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -2267,7 +2268,7 @@
         <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
@@ -2277,12 +2278,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -2297,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H39" t="s">
         <v>45</v>
@@ -2307,12 +2308,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -2327,7 +2328,7 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H40" t="s">
         <v>45</v>
@@ -2337,12 +2338,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -2357,7 +2358,7 @@
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H41" t="s">
         <v>46</v>
@@ -2367,12 +2368,12 @@
         <v>Effect (task non-satisfying)</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -2387,7 +2388,7 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H42" t="s">
         <v>42</v>
@@ -2397,12 +2398,12 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -2417,7 +2418,7 @@
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H43" t="s">
         <v>42</v>
@@ -2427,12 +2428,12 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -2447,7 +2448,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -2457,12 +2458,12 @@
         <v>Pre-Effect</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C45">
         <v>13</v>
@@ -2477,7 +2478,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2487,12 +2488,12 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -2507,7 +2508,7 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -2517,12 +2518,12 @@
         <v>Pre-Quality</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -2537,7 +2538,7 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H47" t="s">
         <v>45</v>
@@ -2547,12 +2548,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C48">
         <v>16</v>
@@ -2567,7 +2568,7 @@
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H48" t="s">
         <v>45</v>
@@ -2577,12 +2578,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2597,7 +2598,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H49" t="s">
         <v>12</v>
@@ -2607,12 +2608,12 @@
         <v>is AND-refined to</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -2627,7 +2628,7 @@
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
@@ -2637,12 +2638,12 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -2657,7 +2658,7 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H51" t="s">
         <v>44</v>
@@ -2667,12 +2668,12 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2687,7 +2688,7 @@
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H52" t="s">
         <v>43</v>
@@ -2697,12 +2698,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -2717,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="G53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H53" t="s">
         <v>43</v>
@@ -2727,12 +2728,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -2747,7 +2748,7 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H54" t="s">
         <v>43</v>
@@ -2757,12 +2758,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C55">
         <v>7</v>
@@ -2777,22 +2778,22 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
         <v>precedes</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C56">
         <v>8</v>
@@ -2807,7 +2808,7 @@
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
@@ -2817,12 +2818,12 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C57">
         <v>9</v>
@@ -2837,7 +2838,7 @@
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H57" t="s">
         <v>50</v>
@@ -2847,12 +2848,12 @@
         <v>positively contributes to</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B58" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -2867,7 +2868,7 @@
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H58" t="s">
         <v>51</v>
@@ -2887,47 +2888,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A67578-F426-48F2-87A8-25344D20072D}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="68.6640625" customWidth="1"/>
     <col min="6" max="7" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2941,10 +2942,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -2953,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2967,10 +2968,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2979,7 +2980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2993,10 +2994,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -3005,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -3019,10 +3020,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -3031,7 +3032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -3045,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -3057,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3071,10 +3072,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -3083,12 +3084,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -3097,10 +3098,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -3109,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3123,10 +3124,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -3135,12 +3136,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -3149,24 +3150,24 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>166</v>
-      </c>
-      <c r="F10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" t="s">
-        <v>167</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3175,10 +3176,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -3187,12 +3188,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3201,10 +3202,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -3213,12 +3214,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3227,10 +3228,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -3239,12 +3240,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3253,10 +3254,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -3265,12 +3266,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3279,10 +3280,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3291,12 +3292,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3305,10 +3306,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -3317,12 +3318,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3331,10 +3332,10 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -3343,12 +3344,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -3357,10 +3358,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -3369,12 +3370,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>123</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -3383,10 +3384,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G19" s="6" t="b">
         <v>1</v>
@@ -3395,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -3403,16 +3404,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="6" t="b">
         <v>0</v>
@@ -3421,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -3429,16 +3430,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G21" s="6" t="b">
         <v>0</v>
@@ -3447,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -3455,16 +3456,16 @@
         <v>3</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G22" s="6" t="b">
         <v>0</v>
@@ -3473,24 +3474,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="6" t="b">
         <v>0</v>
@@ -3499,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -3507,42 +3508,42 @@
         <v>6</v>
       </c>
       <c r="C24" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="D24" s="6">
-        <v>1</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="D25" s="6">
         <v>2</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G25" s="6" t="b">
         <v>1</v>
@@ -3551,24 +3552,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="6" t="b">
         <v>1</v>
@@ -3577,24 +3578,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G27" s="6" t="b">
         <v>1</v>
@@ -3603,24 +3604,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G28" s="6" t="b">
         <v>1</v>
@@ -3629,24 +3630,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G29" s="6" t="b">
         <v>1</v>
@@ -3655,24 +3656,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="C30" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D30" s="6">
         <v>2</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G30" s="6" t="b">
         <v>1</v>
@@ -3681,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3737,7 +3738,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -3793,7 +3794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -3821,7 +3822,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -3849,7 +3850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3933,7 +3934,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -3961,7 +3962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -4009,28 +4010,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2213172F-6AC1-42CA-8EAF-DBEE6814A5DB}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>68</v>
@@ -4050,28 +4051,28 @@
         <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4079,7 +4080,7 @@
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
@@ -4088,31 +4089,31 @@
         <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" t="s">
         <v>127</v>
       </c>
-      <c r="I2" t="s">
-        <v>128</v>
-      </c>
       <c r="J2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -4120,7 +4121,7 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>57</v>
@@ -4132,15 +4133,15 @@
         <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" location="concepts" xr:uid="{645C2665-383D-484E-9957-CE3D12BF6C43}"/>
-    <hyperlink ref="E3" r:id="rId2" location="relationships" xr:uid="{BA3666BF-2274-4326-88B8-21AF91870A99}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{3CE29231-E3FA-45A8-AFE3-276D74CD3008}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{BE7ADA23-5AED-4259-8874-ACDC0712E9D6}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{3CE29231-E3FA-45A8-AFE3-276D74CD3008}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{BE7ADA23-5AED-4259-8874-ACDC0712E9D6}"/>
+    <hyperlink ref="E3" r:id="rId4" location="relationships" xr:uid="{BA3666BF-2274-4326-88B8-21AF91870A99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -4151,24 +4152,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77FB8ED-296C-4040-BCEE-A5690B45B944}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="128.7109375" customWidth="1"/>
+    <col min="3" max="3" width="128.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="69.140625" customWidth="1"/>
-    <col min="6" max="6" width="66.7109375" customWidth="1"/>
+    <col min="5" max="5" width="69.109375" customWidth="1"/>
+    <col min="6" max="6" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
         <v>72</v>
@@ -4186,7 +4187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="187.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -4194,36 +4195,36 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="210.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="270" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>222</v>
@@ -4245,13 +4246,13 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -4259,39 +4260,39 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -4299,25 +4300,25 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>

</xml_diff>